<commit_message>
Relatório Atualizado e Enviado Para Avaliação
</commit_message>
<xml_diff>
--- a/Acessibilidade/relatorios/relatorio_principal.xlsx
+++ b/Acessibilidade/relatorios/relatorio_principal.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UwAmp\www\2sem_prj_integrador\Acessibilidade\relatorios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB872B3-7269-4E7F-A9E0-8BAEFFD0B7D7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6B8CAA-2420-49DC-92C6-C6682EF09A8B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Relatorio" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Legenda" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Relatorio!$A$1:$O$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Relatorio'!$A$1:$O$23</definedName>
     <definedName name="Gravidade">Legenda!$B$2:$B$4</definedName>
     <definedName name="Status">Legenda!$B$7:$B$10</definedName>
   </definedNames>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="166">
   <si>
     <t>ID</t>
   </si>
@@ -1285,10 +1285,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3284,8 +3284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="15" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="J2" s="16">
         <v>43341</v>
@@ -3398,7 +3398,9 @@
       <c r="N2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="17"/>
+      <c r="O2" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
       <c r="R2" s="22"/>
@@ -3427,7 +3429,7 @@
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="15" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="J3" s="19" t="s">
         <v>29</v>
@@ -3444,7 +3446,9 @@
       <c r="N3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="10"/>
+      <c r="O3" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="P3" s="23"/>
       <c r="Q3" s="23"/>
       <c r="R3" s="23"/>
@@ -3659,7 +3663,7 @@
         <v>63</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="J8" s="16">
         <v>43341</v>
@@ -3674,7 +3678,9 @@
       <c r="N8" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="O8" s="17"/>
+      <c r="O8" s="17" t="s">
+        <v>76</v>
+      </c>
       <c r="P8" s="22"/>
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
@@ -3705,7 +3711,7 @@
         <v>63</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="J9" s="19">
         <v>43342</v>
@@ -3718,7 +3724,9 @@
       <c r="N9" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="O9" s="10"/>
+      <c r="O9" s="10" t="s">
+        <v>76</v>
+      </c>
       <c r="P9" s="23"/>
       <c r="Q9" s="23"/>
       <c r="R9" s="23"/>
@@ -3749,7 +3757,7 @@
         <v>70</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="J10" s="16">
         <v>43343</v>
@@ -3762,7 +3770,9 @@
       <c r="N10" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="O10" s="17"/>
+      <c r="O10" s="17" t="s">
+        <v>76</v>
+      </c>
       <c r="P10" s="22"/>
       <c r="Q10" s="22"/>
       <c r="R10" s="22"/>
@@ -3793,7 +3803,7 @@
         <v>150</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="J11" s="16">
         <v>43373</v>
@@ -4707,7 +4717,7 @@
       </c>
       <c r="L32" s="37"/>
       <c r="M32" s="37"/>
-      <c r="N32" s="37" t="s">
+      <c r="N32" s="39" t="s">
         <v>65</v>
       </c>
       <c r="O32" s="37"/>
@@ -4748,7 +4758,7 @@
       </c>
       <c r="L33" s="37"/>
       <c r="M33" s="37"/>
-      <c r="N33" s="37" t="s">
+      <c r="N33" s="39" t="s">
         <v>65</v>
       </c>
       <c r="O33" s="37"/>
@@ -4789,7 +4799,7 @@
       </c>
       <c r="L34" s="17"/>
       <c r="M34" s="10"/>
-      <c r="N34" s="37" t="s">
+      <c r="N34" s="39" t="s">
         <v>65</v>
       </c>
       <c r="O34" s="17"/>
@@ -5402,14 +5412,14 @@
         <v>80</v>
       </c>
       <c r="B2" s="26">
-        <f>COUNTIF(Relatorio!I2:I65,"Corrigido")</f>
-        <v>0</v>
+        <f>COUNTIF('Relatorio'!I2:I65,"Corrigido")</f>
+        <v>6</v>
       </c>
       <c r="F2" s="34" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="26">
-        <f>COUNTIF(Relatorio!F2:F65,"Crítico")</f>
+        <f>COUNTIF('Relatorio'!F2:F65,"Crítico")</f>
         <v>10</v>
       </c>
     </row>
@@ -5418,14 +5428,14 @@
         <v>21</v>
       </c>
       <c r="B3" s="26">
-        <f>COUNTIF(Relatorio!I2:I65,"Atribuído")</f>
-        <v>33</v>
+        <f>COUNTIF('Relatorio'!I2:I65,"Atribuído")</f>
+        <v>27</v>
       </c>
       <c r="F3" s="35" t="s">
         <v>42</v>
       </c>
       <c r="G3" s="26">
-        <f>COUNTIF(Relatorio!F2:F65,"Moderado")</f>
+        <f>COUNTIF('Relatorio'!F2:F65,"Moderado")</f>
         <v>21</v>
       </c>
     </row>
@@ -5434,14 +5444,14 @@
         <v>57</v>
       </c>
       <c r="B4" s="26">
-        <f>COUNTIF(Relatorio!I2:I65,"Não Atribuído")</f>
+        <f>COUNTIF('Relatorio'!I2:I65,"Não Atribuído")</f>
         <v>0</v>
       </c>
       <c r="F4" s="36" t="s">
         <v>35</v>
       </c>
       <c r="G4" s="26">
-        <f>COUNTIF(Relatorio!F2:F65,"Leve")</f>
+        <f>COUNTIF('Relatorio'!F2:F65,"Leve")</f>
         <v>2</v>
       </c>
     </row>
@@ -5450,7 +5460,7 @@
         <v>139</v>
       </c>
       <c r="B5" s="26">
-        <f>COUNTIF(Relatorio!I5:I68,"Sem Ação")</f>
+        <f>COUNTIF('Relatorio'!I5:I68,"Sem Ação")</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>